<commit_message>
Create Suggestion Player Test for Part 2 Fails without errors
</commit_message>
<xml_diff>
--- a/ourboardfiles/Planning_Board_Spreadsheet.xlsx
+++ b/ourboardfiles/Planning_Board_Spreadsheet.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -131,11 +130,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
-  </numFmts>
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -144,22 +140,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="36"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -213,7 +194,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -221,77 +202,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="4" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="5" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="6" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -350,29 +279,325 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF26"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="29" zoomScaleNormal="29" zoomScalePageLayoutView="100">
-      <selection activeCell="AG24" activeCellId="0" pane="topLeft" sqref="AG24"/>
+    <sheetView tabSelected="1" zoomScale="29" zoomScaleNormal="29" workbookViewId="0">
+      <selection activeCell="AG24" sqref="AG24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="25" min="1" style="0" width="12.7125506072875"/>
-    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="8.5748987854251"/>
+    <col min="1" max="25" width="12.7109375"/>
+    <col min="26" max="26" width="10" bestFit="1" customWidth="1"/>
+    <col min="27" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="39.95" outlineLevel="0" r="1">
+    <row r="1" spans="1:32" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -448,11 +673,11 @@
       <c r="Y1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="Z1" s="4" t="n">
+      <c r="Z1" s="4">
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="39.95" outlineLevel="0" r="2">
+    <row r="2" spans="1:32" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -528,7 +753,7 @@
       <c r="Y2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="Z2" s="4" t="n">
+      <c r="Z2" s="4">
         <v>1</v>
       </c>
       <c r="AA2" s="5" t="s">
@@ -542,7 +767,7 @@
       <c r="AE2" s="6"/>
       <c r="AF2" s="6"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="39.95" outlineLevel="0" r="3">
+    <row r="3" spans="1:32" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -618,7 +843,7 @@
       <c r="Y3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="Z3" s="4" t="n">
+      <c r="Z3" s="4">
         <v>2</v>
       </c>
       <c r="AA3" s="5" t="s">
@@ -632,7 +857,7 @@
       <c r="AE3" s="6"/>
       <c r="AF3" s="6"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="39.95" outlineLevel="0" r="4">
+    <row r="4" spans="1:32" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -708,7 +933,7 @@
       <c r="Y4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="Z4" s="4" t="n">
+      <c r="Z4" s="4">
         <v>3</v>
       </c>
       <c r="AA4" s="5" t="s">
@@ -722,7 +947,7 @@
       <c r="AE4" s="6"/>
       <c r="AF4" s="6"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="39.95" outlineLevel="0" r="5">
+    <row r="5" spans="1:32" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
@@ -798,7 +1023,7 @@
       <c r="Y5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="Z5" s="4" t="n">
+      <c r="Z5" s="4">
         <v>4</v>
       </c>
       <c r="AA5" s="5" t="s">
@@ -812,7 +1037,7 @@
       <c r="AE5" s="6"/>
       <c r="AF5" s="6"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="39.95" outlineLevel="0" r="6">
+    <row r="6" spans="1:32" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
@@ -888,7 +1113,7 @@
       <c r="Y6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="Z6" s="4" t="n">
+      <c r="Z6" s="4">
         <v>5</v>
       </c>
       <c r="AA6" s="5" t="s">
@@ -902,7 +1127,7 @@
       <c r="AE6" s="6"/>
       <c r="AF6" s="6"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="39.95" outlineLevel="0" r="7">
+    <row r="7" spans="1:32" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -978,7 +1203,7 @@
       <c r="Y7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="Z7" s="4" t="n">
+      <c r="Z7" s="4">
         <v>6</v>
       </c>
       <c r="AA7" s="5" t="s">
@@ -992,7 +1217,7 @@
       <c r="AE7" s="6"/>
       <c r="AF7" s="6"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="39.95" outlineLevel="0" r="8">
+    <row r="8" spans="1:32" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -1068,7 +1293,7 @@
       <c r="Y8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Z8" s="4" t="n">
+      <c r="Z8" s="4">
         <v>7</v>
       </c>
       <c r="AA8" s="5" t="s">
@@ -1082,7 +1307,7 @@
       <c r="AE8" s="6"/>
       <c r="AF8" s="6"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="39.95" outlineLevel="0" r="9">
+    <row r="9" spans="1:32" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -1158,7 +1383,7 @@
       <c r="Y9" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="Z9" s="4" t="n">
+      <c r="Z9" s="4">
         <v>8</v>
       </c>
       <c r="AA9" s="5" t="s">
@@ -1172,7 +1397,7 @@
       <c r="AE9" s="6"/>
       <c r="AF9" s="6"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="39.95" outlineLevel="0" r="10">
+    <row r="10" spans="1:32" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -1248,7 +1473,7 @@
       <c r="Y10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Z10" s="4" t="n">
+      <c r="Z10" s="4">
         <v>9</v>
       </c>
       <c r="AA10" s="5" t="s">
@@ -1262,7 +1487,7 @@
       <c r="AE10" s="6"/>
       <c r="AF10" s="6"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="39.95" outlineLevel="0" r="11">
+    <row r="11" spans="1:32" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -1338,7 +1563,7 @@
       <c r="Y11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Z11" s="4" t="n">
+      <c r="Z11" s="4">
         <v>10</v>
       </c>
       <c r="AA11" s="5" t="s">
@@ -1352,7 +1577,7 @@
       <c r="AE11" s="6"/>
       <c r="AF11" s="6"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="39.95" outlineLevel="0" r="12">
+    <row r="12" spans="1:32" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1428,7 +1653,7 @@
       <c r="Y12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Z12" s="4" t="n">
+      <c r="Z12" s="4">
         <v>11</v>
       </c>
       <c r="AA12" s="5" t="s">
@@ -1442,7 +1667,7 @@
       <c r="AE12" s="6"/>
       <c r="AF12" s="6"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="39.95" outlineLevel="0" r="13">
+    <row r="13" spans="1:32" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A13" s="3" t="s">
         <v>2</v>
       </c>
@@ -1518,7 +1743,7 @@
       <c r="Y13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Z13" s="4" t="n">
+      <c r="Z13" s="4">
         <v>12</v>
       </c>
       <c r="AA13" s="5" t="s">
@@ -1532,7 +1757,7 @@
       <c r="AE13" s="6"/>
       <c r="AF13" s="6"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="39.95" outlineLevel="0" r="14">
+    <row r="14" spans="1:32" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
@@ -1608,7 +1833,7 @@
       <c r="Y14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Z14" s="4" t="n">
+      <c r="Z14" s="4">
         <v>13</v>
       </c>
       <c r="AA14" s="5"/>
@@ -1618,7 +1843,7 @@
       <c r="AE14" s="6"/>
       <c r="AF14" s="6"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="39.95" outlineLevel="0" r="15">
+    <row r="15" spans="1:32" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
@@ -1694,11 +1919,11 @@
       <c r="Y15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Z15" s="4" t="n">
+      <c r="Z15" s="4">
         <v>14</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="39.95" outlineLevel="0" r="16">
+    <row r="16" spans="1:32" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -1774,11 +1999,11 @@
       <c r="Y16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Z16" s="4" t="n">
+      <c r="Z16" s="4">
         <v>15</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="39.95" outlineLevel="0" r="17">
+    <row r="17" spans="1:26" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -1854,11 +2079,11 @@
       <c r="Y17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Z17" s="4" t="n">
+      <c r="Z17" s="4">
         <v>16</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="39.95" outlineLevel="0" r="18">
+    <row r="18" spans="1:26" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -1934,11 +2159,11 @@
       <c r="Y18" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="Z18" s="4" t="n">
+      <c r="Z18" s="4">
         <v>17</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="39.95" outlineLevel="0" r="19">
+    <row r="19" spans="1:26" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A19" s="3" t="s">
         <v>2</v>
       </c>
@@ -2014,11 +2239,11 @@
       <c r="Y19" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Z19" s="4" t="n">
+      <c r="Z19" s="4">
         <v>18</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="39.95" outlineLevel="0" r="20">
+    <row r="20" spans="1:26" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A20" s="2" t="s">
         <v>1</v>
       </c>
@@ -2094,11 +2319,11 @@
       <c r="Y20" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="Z20" s="4" t="n">
+      <c r="Z20" s="4">
         <v>19</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="39.95" outlineLevel="0" r="21">
+    <row r="21" spans="1:26" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
@@ -2174,11 +2399,11 @@
       <c r="Y21" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="Z21" s="4" t="n">
+      <c r="Z21" s="4">
         <v>20</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="39.95" outlineLevel="0" r="22">
+    <row r="22" spans="1:26" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A22" s="1" t="s">
         <v>18</v>
       </c>
@@ -2254,11 +2479,11 @@
       <c r="Y22" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="Z22" s="4" t="n">
+      <c r="Z22" s="4">
         <v>21</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="39.95" outlineLevel="0" r="23">
+    <row r="23" spans="1:26" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A23" s="1" t="s">
         <v>18</v>
       </c>
@@ -2334,11 +2559,11 @@
       <c r="Y23" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="Z23" s="4" t="n">
+      <c r="Z23" s="4">
         <v>22</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="39.95" outlineLevel="0" r="24">
+    <row r="24" spans="1:26" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A24" s="1" t="s">
         <v>18</v>
       </c>
@@ -2414,11 +2639,11 @@
       <c r="Y24" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="Z24" s="4" t="n">
+      <c r="Z24" s="4">
         <v>23</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="39.95" outlineLevel="0" r="25">
+    <row r="25" spans="1:26" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A25" s="1" t="s">
         <v>18</v>
       </c>
@@ -2494,94 +2719,89 @@
       <c r="Y25" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="Z25" s="4" t="n">
+      <c r="Z25" s="4">
         <v>24</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="48.85" outlineLevel="0" r="26">
-      <c r="A26" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="B26" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C26" s="4" t="n">
+    <row r="26" spans="1:26" ht="48.95" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A26" s="4">
+        <v>0</v>
+      </c>
+      <c r="B26" s="4">
+        <v>1</v>
+      </c>
+      <c r="C26" s="4">
         <v>2</v>
       </c>
-      <c r="D26" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="E26" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="F26" s="4" t="n">
+      <c r="D26" s="4">
+        <v>3</v>
+      </c>
+      <c r="E26" s="4">
+        <v>4</v>
+      </c>
+      <c r="F26" s="4">
         <v>5</v>
       </c>
-      <c r="G26" s="4" t="n">
+      <c r="G26" s="4">
         <v>6</v>
       </c>
-      <c r="H26" s="4" t="n">
+      <c r="H26" s="4">
         <v>7</v>
       </c>
-      <c r="I26" s="4" t="n">
+      <c r="I26" s="4">
         <v>8</v>
       </c>
-      <c r="J26" s="4" t="n">
+      <c r="J26" s="4">
         <v>9</v>
       </c>
-      <c r="K26" s="4" t="n">
-        <v>10</v>
-      </c>
-      <c r="L26" s="4" t="n">
+      <c r="K26" s="4">
+        <v>10</v>
+      </c>
+      <c r="L26" s="4">
         <v>11</v>
       </c>
-      <c r="M26" s="4" t="n">
+      <c r="M26" s="4">
         <v>12</v>
       </c>
-      <c r="N26" s="4" t="n">
-        <v>13</v>
-      </c>
-      <c r="O26" s="4" t="n">
+      <c r="N26" s="4">
+        <v>13</v>
+      </c>
+      <c r="O26" s="4">
         <v>14</v>
       </c>
-      <c r="P26" s="4" t="n">
+      <c r="P26" s="4">
         <v>15</v>
       </c>
-      <c r="Q26" s="4" t="n">
-        <v>16</v>
-      </c>
-      <c r="R26" s="4" t="n">
+      <c r="Q26" s="4">
+        <v>16</v>
+      </c>
+      <c r="R26" s="4">
         <v>17</v>
       </c>
-      <c r="S26" s="4" t="n">
-        <v>18</v>
-      </c>
-      <c r="T26" s="4" t="n">
+      <c r="S26" s="4">
+        <v>18</v>
+      </c>
+      <c r="T26" s="4">
         <v>19</v>
       </c>
-      <c r="U26" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="V26" s="4" t="n">
+      <c r="U26" s="4">
+        <v>20</v>
+      </c>
+      <c r="V26" s="4">
         <v>21</v>
       </c>
-      <c r="W26" s="4" t="n">
+      <c r="W26" s="4">
         <v>22</v>
       </c>
-      <c r="X26" s="4" t="n">
-        <v>23</v>
-      </c>
-      <c r="Y26" s="4" t="n">
+      <c r="X26" s="4">
+        <v>23</v>
+      </c>
+      <c r="Y26" s="4">
         <v>24</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
officially committing git log so merge can occur
</commit_message>
<xml_diff>
--- a/ourboardfiles/Planning_Board_Spreadsheet.xlsx
+++ b/ourboardfiles/Planning_Board_Spreadsheet.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -131,11 +130,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
-  </numFmts>
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -144,22 +140,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="36"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -213,7 +194,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -221,77 +202,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="4" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="5" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="6" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -350,29 +279,325 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF26"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="29" zoomScaleNormal="29" zoomScalePageLayoutView="100">
-      <selection activeCell="AG24" activeCellId="0" pane="topLeft" sqref="AG24"/>
+    <sheetView tabSelected="1" zoomScale="29" zoomScaleNormal="29" workbookViewId="0">
+      <selection activeCell="AG24" sqref="AG24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="25" min="1" style="0" width="12.7125506072875"/>
-    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="8.5748987854251"/>
+    <col min="1" max="25" width="12.7109375"/>
+    <col min="26" max="26" width="10" bestFit="1" customWidth="1"/>
+    <col min="27" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="39.95" outlineLevel="0" r="1">
+    <row r="1" spans="1:32" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -448,11 +673,11 @@
       <c r="Y1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="Z1" s="4" t="n">
+      <c r="Z1" s="4">
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="39.95" outlineLevel="0" r="2">
+    <row r="2" spans="1:32" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -528,7 +753,7 @@
       <c r="Y2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="Z2" s="4" t="n">
+      <c r="Z2" s="4">
         <v>1</v>
       </c>
       <c r="AA2" s="5" t="s">
@@ -542,7 +767,7 @@
       <c r="AE2" s="6"/>
       <c r="AF2" s="6"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="39.95" outlineLevel="0" r="3">
+    <row r="3" spans="1:32" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -618,7 +843,7 @@
       <c r="Y3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="Z3" s="4" t="n">
+      <c r="Z3" s="4">
         <v>2</v>
       </c>
       <c r="AA3" s="5" t="s">
@@ -632,7 +857,7 @@
       <c r="AE3" s="6"/>
       <c r="AF3" s="6"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="39.95" outlineLevel="0" r="4">
+    <row r="4" spans="1:32" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -708,7 +933,7 @@
       <c r="Y4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="Z4" s="4" t="n">
+      <c r="Z4" s="4">
         <v>3</v>
       </c>
       <c r="AA4" s="5" t="s">
@@ -722,7 +947,7 @@
       <c r="AE4" s="6"/>
       <c r="AF4" s="6"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="39.95" outlineLevel="0" r="5">
+    <row r="5" spans="1:32" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
@@ -798,7 +1023,7 @@
       <c r="Y5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="Z5" s="4" t="n">
+      <c r="Z5" s="4">
         <v>4</v>
       </c>
       <c r="AA5" s="5" t="s">
@@ -812,7 +1037,7 @@
       <c r="AE5" s="6"/>
       <c r="AF5" s="6"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="39.95" outlineLevel="0" r="6">
+    <row r="6" spans="1:32" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
@@ -888,7 +1113,7 @@
       <c r="Y6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="Z6" s="4" t="n">
+      <c r="Z6" s="4">
         <v>5</v>
       </c>
       <c r="AA6" s="5" t="s">
@@ -902,7 +1127,7 @@
       <c r="AE6" s="6"/>
       <c r="AF6" s="6"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="39.95" outlineLevel="0" r="7">
+    <row r="7" spans="1:32" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -978,7 +1203,7 @@
       <c r="Y7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="Z7" s="4" t="n">
+      <c r="Z7" s="4">
         <v>6</v>
       </c>
       <c r="AA7" s="5" t="s">
@@ -992,7 +1217,7 @@
       <c r="AE7" s="6"/>
       <c r="AF7" s="6"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="39.95" outlineLevel="0" r="8">
+    <row r="8" spans="1:32" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -1068,7 +1293,7 @@
       <c r="Y8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Z8" s="4" t="n">
+      <c r="Z8" s="4">
         <v>7</v>
       </c>
       <c r="AA8" s="5" t="s">
@@ -1082,7 +1307,7 @@
       <c r="AE8" s="6"/>
       <c r="AF8" s="6"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="39.95" outlineLevel="0" r="9">
+    <row r="9" spans="1:32" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -1158,7 +1383,7 @@
       <c r="Y9" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="Z9" s="4" t="n">
+      <c r="Z9" s="4">
         <v>8</v>
       </c>
       <c r="AA9" s="5" t="s">
@@ -1172,7 +1397,7 @@
       <c r="AE9" s="6"/>
       <c r="AF9" s="6"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="39.95" outlineLevel="0" r="10">
+    <row r="10" spans="1:32" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -1248,7 +1473,7 @@
       <c r="Y10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Z10" s="4" t="n">
+      <c r="Z10" s="4">
         <v>9</v>
       </c>
       <c r="AA10" s="5" t="s">
@@ -1262,7 +1487,7 @@
       <c r="AE10" s="6"/>
       <c r="AF10" s="6"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="39.95" outlineLevel="0" r="11">
+    <row r="11" spans="1:32" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -1338,7 +1563,7 @@
       <c r="Y11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Z11" s="4" t="n">
+      <c r="Z11" s="4">
         <v>10</v>
       </c>
       <c r="AA11" s="5" t="s">
@@ -1352,7 +1577,7 @@
       <c r="AE11" s="6"/>
       <c r="AF11" s="6"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="39.95" outlineLevel="0" r="12">
+    <row r="12" spans="1:32" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1428,7 +1653,7 @@
       <c r="Y12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Z12" s="4" t="n">
+      <c r="Z12" s="4">
         <v>11</v>
       </c>
       <c r="AA12" s="5" t="s">
@@ -1442,7 +1667,7 @@
       <c r="AE12" s="6"/>
       <c r="AF12" s="6"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="39.95" outlineLevel="0" r="13">
+    <row r="13" spans="1:32" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A13" s="3" t="s">
         <v>2</v>
       </c>
@@ -1518,7 +1743,7 @@
       <c r="Y13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Z13" s="4" t="n">
+      <c r="Z13" s="4">
         <v>12</v>
       </c>
       <c r="AA13" s="5" t="s">
@@ -1532,7 +1757,7 @@
       <c r="AE13" s="6"/>
       <c r="AF13" s="6"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="39.95" outlineLevel="0" r="14">
+    <row r="14" spans="1:32" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
@@ -1608,7 +1833,7 @@
       <c r="Y14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Z14" s="4" t="n">
+      <c r="Z14" s="4">
         <v>13</v>
       </c>
       <c r="AA14" s="5"/>
@@ -1618,7 +1843,7 @@
       <c r="AE14" s="6"/>
       <c r="AF14" s="6"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="39.95" outlineLevel="0" r="15">
+    <row r="15" spans="1:32" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
@@ -1694,11 +1919,11 @@
       <c r="Y15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Z15" s="4" t="n">
+      <c r="Z15" s="4">
         <v>14</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="39.95" outlineLevel="0" r="16">
+    <row r="16" spans="1:32" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -1774,11 +1999,11 @@
       <c r="Y16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Z16" s="4" t="n">
+      <c r="Z16" s="4">
         <v>15</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="39.95" outlineLevel="0" r="17">
+    <row r="17" spans="1:26" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -1854,11 +2079,11 @@
       <c r="Y17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Z17" s="4" t="n">
+      <c r="Z17" s="4">
         <v>16</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="39.95" outlineLevel="0" r="18">
+    <row r="18" spans="1:26" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -1934,11 +2159,11 @@
       <c r="Y18" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="Z18" s="4" t="n">
+      <c r="Z18" s="4">
         <v>17</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="39.95" outlineLevel="0" r="19">
+    <row r="19" spans="1:26" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A19" s="3" t="s">
         <v>2</v>
       </c>
@@ -2014,11 +2239,11 @@
       <c r="Y19" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Z19" s="4" t="n">
+      <c r="Z19" s="4">
         <v>18</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="39.95" outlineLevel="0" r="20">
+    <row r="20" spans="1:26" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A20" s="2" t="s">
         <v>1</v>
       </c>
@@ -2094,11 +2319,11 @@
       <c r="Y20" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="Z20" s="4" t="n">
+      <c r="Z20" s="4">
         <v>19</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="39.95" outlineLevel="0" r="21">
+    <row r="21" spans="1:26" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
@@ -2174,11 +2399,11 @@
       <c r="Y21" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="Z21" s="4" t="n">
+      <c r="Z21" s="4">
         <v>20</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="39.95" outlineLevel="0" r="22">
+    <row r="22" spans="1:26" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A22" s="1" t="s">
         <v>18</v>
       </c>
@@ -2254,11 +2479,11 @@
       <c r="Y22" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="Z22" s="4" t="n">
+      <c r="Z22" s="4">
         <v>21</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="39.95" outlineLevel="0" r="23">
+    <row r="23" spans="1:26" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A23" s="1" t="s">
         <v>18</v>
       </c>
@@ -2334,11 +2559,11 @@
       <c r="Y23" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="Z23" s="4" t="n">
+      <c r="Z23" s="4">
         <v>22</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="39.95" outlineLevel="0" r="24">
+    <row r="24" spans="1:26" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A24" s="1" t="s">
         <v>18</v>
       </c>
@@ -2414,11 +2639,11 @@
       <c r="Y24" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="Z24" s="4" t="n">
+      <c r="Z24" s="4">
         <v>23</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="39.95" outlineLevel="0" r="25">
+    <row r="25" spans="1:26" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A25" s="1" t="s">
         <v>18</v>
       </c>
@@ -2494,94 +2719,89 @@
       <c r="Y25" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="Z25" s="4" t="n">
+      <c r="Z25" s="4">
         <v>24</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="48.85" outlineLevel="0" r="26">
-      <c r="A26" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="B26" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C26" s="4" t="n">
+    <row r="26" spans="1:26" ht="48.95" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A26" s="4">
+        <v>0</v>
+      </c>
+      <c r="B26" s="4">
+        <v>1</v>
+      </c>
+      <c r="C26" s="4">
         <v>2</v>
       </c>
-      <c r="D26" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="E26" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="F26" s="4" t="n">
+      <c r="D26" s="4">
+        <v>3</v>
+      </c>
+      <c r="E26" s="4">
+        <v>4</v>
+      </c>
+      <c r="F26" s="4">
         <v>5</v>
       </c>
-      <c r="G26" s="4" t="n">
+      <c r="G26" s="4">
         <v>6</v>
       </c>
-      <c r="H26" s="4" t="n">
+      <c r="H26" s="4">
         <v>7</v>
       </c>
-      <c r="I26" s="4" t="n">
+      <c r="I26" s="4">
         <v>8</v>
       </c>
-      <c r="J26" s="4" t="n">
+      <c r="J26" s="4">
         <v>9</v>
       </c>
-      <c r="K26" s="4" t="n">
-        <v>10</v>
-      </c>
-      <c r="L26" s="4" t="n">
+      <c r="K26" s="4">
+        <v>10</v>
+      </c>
+      <c r="L26" s="4">
         <v>11</v>
       </c>
-      <c r="M26" s="4" t="n">
+      <c r="M26" s="4">
         <v>12</v>
       </c>
-      <c r="N26" s="4" t="n">
-        <v>13</v>
-      </c>
-      <c r="O26" s="4" t="n">
+      <c r="N26" s="4">
+        <v>13</v>
+      </c>
+      <c r="O26" s="4">
         <v>14</v>
       </c>
-      <c r="P26" s="4" t="n">
+      <c r="P26" s="4">
         <v>15</v>
       </c>
-      <c r="Q26" s="4" t="n">
-        <v>16</v>
-      </c>
-      <c r="R26" s="4" t="n">
+      <c r="Q26" s="4">
+        <v>16</v>
+      </c>
+      <c r="R26" s="4">
         <v>17</v>
       </c>
-      <c r="S26" s="4" t="n">
-        <v>18</v>
-      </c>
-      <c r="T26" s="4" t="n">
+      <c r="S26" s="4">
+        <v>18</v>
+      </c>
+      <c r="T26" s="4">
         <v>19</v>
       </c>
-      <c r="U26" s="4" t="n">
-        <v>20</v>
-      </c>
-      <c r="V26" s="4" t="n">
+      <c r="U26" s="4">
+        <v>20</v>
+      </c>
+      <c r="V26" s="4">
         <v>21</v>
       </c>
-      <c r="W26" s="4" t="n">
+      <c r="W26" s="4">
         <v>22</v>
       </c>
-      <c r="X26" s="4" t="n">
-        <v>23</v>
-      </c>
-      <c r="Y26" s="4" t="n">
+      <c r="X26" s="4">
+        <v>23</v>
+      </c>
+      <c r="Y26" s="4">
         <v>24</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>